<commit_message>
correlate wwo and ogimet with hot and cool seasons
</commit_message>
<xml_diff>
--- a/correlation_summary_wwo.xlsx
+++ b/correlation_summary_wwo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\COLLEGE FILES\THESIS\correlation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B7B00-F9D8-4BA2-AADB-3C1EF839920A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCED240-570C-467F-9327-B52898DD5CAB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" tabRatio="816" activeTab="4" xr2:uid="{590F9863-D67A-4092-8D1A-1440B82F5E82}"/>
   </bookViews>
@@ -9051,7 +9051,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9113,49 +9113,49 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>0.26279764784569998</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>-0.28323960303178097</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>-0.12668700795895199</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>-0.20801548279632001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>1.01871272900811E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>0.31272011579255199</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>-2.5115026441127002E-2</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>-6.2759708858418903E-2</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>4.1358172855785601E-2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>-0.25179757761527</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>1.1421775416918901E-2</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>-0.28316796930525401</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>-7.3284256157308603E-2</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>-0.25180803301883797</v>
       </c>
     </row>
@@ -9166,49 +9166,49 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.26279764784569998</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>-0.12838874171761</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>-0.10752250684051699</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>-2.37408445297747E-3</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>-6.1413564249245801E-2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.148899222629408</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>6.8509994185723594E-2</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>4.55956508212981E-2</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>4.3506801282394203E-2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>-0.101243263875449</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>2.6311072294377898E-2</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>-0.128287190671312</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>-0.101270932920017</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="1">
         <v>-0.101211173395804</v>
       </c>
     </row>
@@ -9219,49 +9219,49 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.56477111441248595</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>-9.1296110451609597E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>2.10928492630592E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>-2.4076266004659199E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>-6.8021665332174103E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>2.4421814023361701E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>4.1456465194612102E-2</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>0.113648147349813</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>-3.8118882749743503E-2</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>-0.11204465382600599</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <v>-0.14474888994608201</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
         <v>-9.1183900117444205E-2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="1">
         <v>2.01785002031925E-2</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="1">
         <v>-0.112042590443979</v>
       </c>
     </row>
@@ -9272,49 +9272,49 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.56477111441248595</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <v>-7.0438067769366203E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1.9521464204320702E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>-6.1164516684916199E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>-5.7682615280295897E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>2.0659232759852E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>5.9715775792315101E-2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>6.9376422246872696E-2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>-1.7241532584784999E-2</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>-8.6671056993219198E-2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>-0.121326805470023</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>-7.0346745600415594E-2</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>1.70575051219862E-2</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="1">
         <v>-8.66755592977978E-2</v>
       </c>
     </row>
@@ -9325,49 +9325,49 @@
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.46577113607791099</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>-0.28158737116885402</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>-0.17837301205311101</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>-0.22752772082157599</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>1.95549361280394E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>0.31017446953891897</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>-2.63800237039402E-2</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>-0.105462661602504</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>4.8965338103603297E-2</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>-0.25491370626115001</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>4.7957906000642902E-3</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>-0.281808082589939</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <v>-0.115208476662871</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="1">
         <v>-0.25492202576909401</v>
       </c>
     </row>
@@ -9378,49 +9378,49 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.46577113607791099</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
         <v>-0.139331602760563</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>-6.3369037249673493E-2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>-0.109591623157602</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>1.33445487817413E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>0.113224749112895</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>-1.1416411159233E-2</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>-9.4248725117925203E-2</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>9.4461850780051208E-3</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1">
         <v>-0.14857123166104799</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <v>-9.3319641410605406E-2</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
         <v>-0.139387664502828</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="1">
         <v>-3.4970890078517801E-2</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="1">
         <v>-0.14859691203706099</v>
       </c>
     </row>
@@ -9431,49 +9431,49 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.50497714341664002</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>-0.34342199270750801</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>-0.115703219256706</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>-0.287995340661377</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>-8.5504558254256596E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>0.31013383353014401</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>5.23565774322651E-2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>5.9239825515049603E-2</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>-1.0231757689591E-2</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>-0.33075947574859998</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>-9.5232109099811696E-2</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <v>-0.34352281450495598</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="1">
         <v>-6.1040571756208799E-2</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="1">
         <v>-0.330768555407005</v>
       </c>
     </row>
@@ -9484,49 +9484,49 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>0.50497714341664002</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>-0.24287078359441</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>-0.119879506256937</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>-0.14553556211136801</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>-0.16473330392690599</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>0.18107369717556701</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>0.13059465858219299</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>0.13541676419323101</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>-9.0255232364635202E-2</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>-0.24834499582839201</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>-0.15180793989945601</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
         <v>-0.24298049538404201</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="1">
         <v>-9.9411779160260394E-2</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="1">
         <v>-0.24833689021469299</v>
       </c>
     </row>
@@ -9537,49 +9537,49 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.16875411302953999</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>-1.8115726206180099E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>-3.1523545284420001E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>2.8672048936899102E-3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>-1.9762114223104098E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>1.04573044800689E-2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>2.6192474652737101E-2</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>-4.2835198743540699E-2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>1.8891803357648399E-2</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>-2.1777578291812601E-2</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>-7.1140230895640703E-3</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <v>-1.8066554061475702E-2</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="1">
         <v>-2.8997755490605698E-2</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="1">
         <v>-2.1809904459188401E-2</v>
       </c>
     </row>
@@ -9590,49 +9590,49 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.16875411302953999</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
         <v>-5.5130499787406598E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>-7.6211917744214999E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>-2.8109053060362599E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>-1.87269298385025E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>4.9196239430442899E-2</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>-3.3978686988603399E-3</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>-2.9288803125092199E-2</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>1.45814448173414E-2</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>-5.6215890960187899E-2</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>-3.0365897525633501E-2</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <v>-5.5280084060485603E-2</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="1">
         <v>-5.5132958416689699E-2</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="1">
         <v>-5.6244790165171803E-2</v>
       </c>
     </row>
@@ -9643,49 +9643,49 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
         <v>0.20213207220985299</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>-1.2221326192664601E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>2.2079356518205001E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>1.11599635967375E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>-3.2079179908944697E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>-4.4899365476181504E-3</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>3.5970442876106803E-2</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="1">
         <v>-7.24421333122018E-3</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>1.19092270099876E-3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="1">
         <v>-8.3933212654995204E-3</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <v>2.6754752450204701E-3</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <v>-1.2154590065524801E-2</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="1">
         <v>1.7735767892884498E-2</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="1">
         <v>-8.3851940420754893E-3</v>
       </c>
     </row>
@@ -9696,49 +9696,49 @@
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>0.20213207220985299</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
         <v>2.0316305903187899E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>9.6743560659259299E-3</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>3.59263339348748E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>-2.0111099314046001E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>-3.13972831504057E-2</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>3.6583086528114102E-2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="1">
         <v>1.8023845413368701E-2</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>-2.8370874547883999E-2</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1">
         <v>1.3406928584952399E-2</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <v>-2.1536646987793201E-2</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <v>2.03962060725188E-2</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="1">
         <v>4.7675572172550798E-3</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="1">
         <v>1.3396385633346299E-2</v>
       </c>
     </row>
@@ -9749,49 +9749,49 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.39112821052668201</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>-4.1996605330089101E-2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>-0.129061545075419</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>6.8688487371677603E-3</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>0.23318763787041</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>0.20994063701393101</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>-0.156047186465638</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>-0.31108493690445899</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>0.21128590492678101</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>1.6511329549153402E-2</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>0.266819068536788</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <v>-4.1987656663944398E-2</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="1">
         <v>-8.5741840749101794E-2</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="1">
         <v>1.6520928022252999E-2</v>
       </c>
     </row>
@@ -9802,49 +9802,49 @@
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>0.39112821052668201</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
         <v>-9.85046233168686E-2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>-4.81850387626543E-2</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>-5.8198154450061698E-2</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>4.5668289080178302E-2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <v>0.102959838090523</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
         <v>-6.9106539423675201E-3</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="1">
         <v>-5.8119962816919203E-2</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1">
         <v>6.9831961075604798E-2</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="1">
         <v>-0.10333281106362401</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <v>-4.6442767934802703E-2</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <v>-9.8485563463630493E-2</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="1">
         <v>-2.2035636615087801E-2</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="1">
         <v>-0.103324331214906</v>
       </c>
     </row>
@@ -9855,49 +9855,49 @@
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
         <v>0.38319822737778098</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>-0.17787297820838399</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>-0.109741871673845</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>-0.17234678507354101</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>2.5419219267882601E-2</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>0.20833582051704999</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <v>-1.22845390865279E-2</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="1">
         <v>-0.11031667366922</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>2.1268722982489802E-2</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="1">
         <v>-0.16516804102166899</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="1">
         <v>9.6288476457897006E-3</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="1">
         <v>-0.17799323338541101</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="1">
         <v>-5.2127520222265397E-2</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="1">
         <v>-0.16515003461521799</v>
       </c>
     </row>
@@ -9908,49 +9908,49 @@
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>0.38319822737778098</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>-0.131163834325457</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>-9.5710706997884504E-2</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>-5.7196141156681798E-2</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>-4.3015034365286697E-2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>0.123943196356593</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>1.9965683282617601E-2</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="1">
         <v>4.3900236738901198E-3</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1">
         <v>-2.0029981797083402E-2</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="1">
         <v>-0.131339577169477</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="1">
         <v>-3.8454047886545502E-2</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="1">
         <v>-0.13110452328744801</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="1">
         <v>-6.6234506652232406E-2</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="1">
         <v>-0.13133679461225001</v>
       </c>
     </row>
@@ -9961,49 +9961,49 @@
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
         <v>0.15247541945467699</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>-1.4338912256799801E-2</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>-3.1902467520331199E-2</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>7.4050179544493701E-3</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>-2.45734702530109E-2</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>1.24475141433819E-2</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>4.2951694101300703E-2</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="1">
         <v>2.64452449116255E-2</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1">
         <v>-6.5295807538450601E-2</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="1">
         <v>-2.2633809832962998E-2</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="1">
         <v>-2.29764256232429E-2</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="1">
         <v>-1.4479982955643801E-2</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="1">
         <v>-3.44784902084804E-2</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="1">
         <v>-2.26217069658977E-2</v>
       </c>
     </row>
@@ -10014,49 +10014,49 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0.15247541945467699</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
         <v>-8.8468294780793905E-2</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>-0.18270358282972099</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>-5.3618206528151897E-3</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>4.5138763494563403E-2</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>0.21591397980632801</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="1">
         <v>-3.0321537203873698E-2</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="1">
         <v>-0.129068556835538</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>0.116267355861395</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="1">
         <v>-3.2584914704560999E-2</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="1">
         <v>0.21855420227095901</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="1">
         <v>-8.8429031493337001E-2</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="1">
         <v>-0.15376774403552501</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="1">
         <v>-3.25624455421673E-2</v>
       </c>
     </row>
@@ -10067,49 +10067,49 @@
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
         <v>-4.0604182289775198E-3</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>-1.32626070828414E-2</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>1.2390370190944799E-2</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>-5.7224381818405397E-2</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <v>4.3572733440441699E-2</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <v>-5.6290799462899903E-3</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="1">
         <v>-1.2484117148930499E-2</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="1">
         <v>-8.0096525019881598E-2</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>5.7630078285461801E-2</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1">
         <v>-2.59679641086774E-2</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <v>-3.6299225503713298E-2</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="1">
         <v>-1.3219998530984701E-2</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="1">
         <v>3.1183261197282999E-2</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="1">
         <v>-2.59681996550662E-2</v>
       </c>
     </row>
@@ -10120,49 +10120,49 @@
       <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>-4.0604182289775198E-3</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
         <v>-4.5840992558804097E-2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>0.10745061402678301</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>-1.10321670127798E-2</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>6.7058311708558596E-2</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <v>6.93718582555911E-3</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
         <v>-4.6644617933965002E-2</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <v>-8.5153566727659297E-3</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <v>7.0485397709150396E-2</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="1">
         <v>-5.3106828498343202E-2</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="1">
         <v>-8.3585876628378505E-2</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="1">
         <v>-4.55808943307765E-2</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="1">
         <v>0.103283986582868</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="1">
         <v>-5.3122851753733998E-2</v>
       </c>
     </row>
@@ -10173,49 +10173,49 @@
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
         <v>0.25298160680943199</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>-9.2960334461670804E-2</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>-3.6679734512044801E-2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>-5.1496818416453198E-2</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>-1.62003898937003E-2</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>4.5799402753785502E-2</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <v>2.6482633283278399E-2</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="1">
         <v>6.0775094751107303E-3</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>8.5496730020167694E-3</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="1">
         <v>-0.11841022829565701</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <v>-0.123457619712091</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="1">
         <v>-9.2891830349277504E-2</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="1">
         <v>-1.3375182992854E-2</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="1">
         <v>-0.118403359135937</v>
       </c>
     </row>
@@ -10226,49 +10226,49 @@
       <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.25298160680943199</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
         <v>-0.219422955447374</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>-0.15673203850730799</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>-7.2012671759954003E-2</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>-2.84894787962305E-2</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>0.19452029032787299</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <v>3.2053878322467998E-2</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="1">
         <v>-7.14858671687743E-3</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>7.2587484799078505E-2</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="1">
         <v>-0.20532434605774499</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="1">
         <v>-4.3599516126694098E-2</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="1">
         <v>-0.21929940654258701</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="1">
         <v>-0.13193070440677801</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="1">
         <v>-0.20531522624065099</v>
       </c>
     </row>
@@ -10279,49 +10279,49 @@
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
         <v>0.36765749142774301</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>-0.114652152048797</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>-0.113337483283119</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>-2.3500408201896399E-2</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1">
         <v>-0.119402776061939</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="1">
         <v>9.3907393858478794E-2</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
         <v>8.9859566201217503E-2</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="1">
         <v>6.2125856915305602E-2</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>-4.6016320947080899E-2</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="1">
         <v>-0.10582472471278</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="1">
         <v>-4.3232206034819302E-2</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="1">
         <v>-0.114902435007553</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="1">
         <v>-0.11381393620420199</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="1">
         <v>-0.105857500728901</v>
       </c>
     </row>
@@ -10332,49 +10332,49 @@
       <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>0.36765749142774301</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
         <v>-0.187733798139714</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>-4.92259202948723E-2</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>-0.14001882743045299</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1">
         <v>2.47721711473699E-2</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
         <v>0.21042790441378201</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
         <v>-2.9916039374543998E-2</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="1">
         <v>-6.0936760969540101E-2</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <v>7.1110083171581101E-2</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="1">
         <v>-0.166128183431107</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="1">
         <v>3.3410878932082599E-3</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="1">
         <v>-0.18797794071423601</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="1">
         <v>-1.09224787654554E-2</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="1">
         <v>-0.166154072761138</v>
       </c>
     </row>
@@ -10385,49 +10385,49 @@
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
         <v>0.45108812395194398</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>-6.2047362241165402E-2</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>-8.9332461988987602E-2</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>-2.2915667761169399E-2</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>4.2953407869502601E-3</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>2.4183292265629201E-2</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <v>2.9053681145142101E-2</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="1">
         <v>-2.4959932356868698E-2</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>2.3935057593077E-2</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1">
         <v>-7.8301731772908098E-2</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <v>-8.7280484869243002E-2</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="1">
         <v>-6.21132715768817E-2</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="1">
         <v>-6.8758324785475694E-2</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="1">
         <v>-7.8288454491680801E-2</v>
       </c>
     </row>
@@ -10438,49 +10438,49 @@
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>0.45108812395194398</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
         <v>-6.7396157186841693E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>-0.114854326872164</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>-3.4863432050658998E-2</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="1">
         <v>2.5237475356132001E-2</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="1">
         <v>7.2312413074318904E-2</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="1">
         <v>-7.2711755289170702E-3</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="1">
         <v>-7.5885660833820895E-2</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <v>3.2073394803395897E-2</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="1">
         <v>-6.6497769142914401E-2</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="1">
         <v>-2.52308819715805E-2</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="1">
         <v>-6.7362197509510002E-2</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="1">
         <v>-8.5420032120052697E-2</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="1">
         <v>-6.6520580503411003E-2</v>
       </c>
     </row>
@@ -10491,49 +10491,49 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
         <v>8.7452215571416303E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>-6.63819879645835E-2</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>-1.4652621133592199E-2</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>-2.36538258035556E-2</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>-5.4269491785870698E-2</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="1">
         <v>2.3327897145917001E-2</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="1">
         <v>6.3768748864449304E-2</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="1">
         <v>5.1137331020039999E-2</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="1">
         <v>-2.3800504613989901E-2</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="1">
         <v>-8.2698805869904607E-2</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="1">
         <v>-8.1017501008475101E-2</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="1">
         <v>-6.6359096237913695E-2</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="1">
         <v>-1.49888077420919E-2</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="1">
         <v>-8.2690141594457395E-2</v>
       </c>
     </row>
@@ -10544,49 +10544,49 @@
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>8.7452215571416303E-2</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
         <v>-6.2950476261820806E-2</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>5.26247510921067E-3</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>-2.0626724402531299E-2</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <v>-7.1316458344319003E-2</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="1">
         <v>9.7701426670954404E-3</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="1">
         <v>5.6512993496245702E-2</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="1">
         <v>6.5000587425274106E-2</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="1">
         <v>2.70746791538462E-2</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="1">
         <v>-8.0933134265282605E-2</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="1">
         <v>-0.106245710332167</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="1">
         <v>-6.2880278515177204E-2</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="1">
         <v>1.4041899231925599E-4</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="1">
         <v>-8.09480187784542E-2</v>
       </c>
     </row>
@@ -10597,49 +10597,49 @@
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
         <v>0.64880610742980305</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>-0.21056485634758201</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>-0.11093667381137599</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>-0.13887010150593099</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1">
         <v>-5.4027001838744301E-2</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="1">
         <v>0.18891813260200899</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
         <v>2.3796188709654401E-2</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="1">
         <v>-2.0491486309083401E-2</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1">
         <v>3.81654526810776E-2</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="1">
         <v>-0.19958786524156699</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="1">
         <v>-6.4306448968243904E-2</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="1">
         <v>-0.21067489119928601</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="1">
         <v>-7.8472920755368103E-2</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="1">
         <v>-0.199601074451839</v>
       </c>
     </row>
@@ -10650,49 +10650,49 @@
       <c r="B31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>0.64880610742980305</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
         <v>-0.25776856946521298</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>-9.2771675396802394E-2</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>-0.223966513637403</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <v>-3.03428965336302E-2</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="1">
         <v>0.24397016654279299</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
         <v>1.2267743092777301E-3</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="1">
         <v>-4.8970664874923901E-2</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <v>5.2621456246766E-2</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="1">
         <v>-0.24442817742936301</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="1">
         <v>-6.2251720620182999E-2</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="1">
         <v>-0.25788920374388402</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="1">
         <v>-4.1822224100856203E-2</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="1">
         <v>-0.244431898981048</v>
       </c>
     </row>
@@ -10703,49 +10703,49 @@
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
         <v>0.57285452904383904</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>-0.23626591842402</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>-6.5319543642334901E-2</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>-8.0045575520882997E-2</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>2.3789657182417502E-3</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>0.22313492263790999</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
         <v>-1.7829054864577001E-2</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="1">
         <v>8.1719921019866703E-3</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <v>0.14785261923755</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="1">
         <v>-0.210108478177259</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="1">
         <v>-1.38614022457949E-2</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="1">
         <v>-0.23647039562642899</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="1">
         <v>-2.9324734981857701E-2</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="1">
         <v>-0.2101014996677</v>
       </c>
     </row>
@@ -10756,49 +10756,49 @@
       <c r="B33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>0.57285452904383904</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
         <v>-0.243725443863678</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>-8.6381395623876506E-2</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>-0.160282155520523</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>1.29398336534562E-2</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="1">
         <v>0.26587166119031302</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
         <v>-2.8044782382913198E-2</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="1">
         <v>-1.9857773939416502E-2</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1">
         <v>0.11768889033222101</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="1">
         <v>-0.20679799898064299</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="1">
         <v>3.7063096311237498E-2</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="1">
         <v>-0.24395094977255</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="1">
         <v>-3.9848383518622597E-2</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="1">
         <v>-0.206799446734482</v>
       </c>
     </row>
@@ -10809,49 +10809,49 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
         <v>0.204074109271492</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>-0.10417176371123101</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>-6.3672694051871898E-2</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>-7.1695803112563294E-2</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>-1.3442452645365199E-2</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="1">
         <v>9.5090961904319593E-2</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
         <v>3.0238698449004901E-2</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="1">
         <v>-3.6836632259355601E-2</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1">
         <v>3.0157794597690398E-3</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="1">
         <v>-9.8094688542759906E-2</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="1">
         <v>-1.9302250342821799E-2</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="1">
         <v>-0.10414736082130099</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="1">
         <v>-4.3722307084062197E-2</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="1">
         <v>-9.8144688622638199E-2</v>
       </c>
     </row>
@@ -10862,49 +10862,49 @@
       <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>0.204074109271492</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>-0.36841314081579302</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>-0.15797935367140201</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>-0.200926716170585</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>-9.5428257864752897E-2</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="1">
         <v>0.35541471292004501</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
         <v>6.9221198437403694E-2</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="1">
         <v>5.1451552120325698E-2</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="1">
         <v>4.5018570914270598E-2</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="1">
         <v>-0.33652196977597498</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="1">
         <v>-3.4189758024732897E-2</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="1">
         <v>-0.36839901891188198</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="1">
         <v>-0.115592650773084</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="1">
         <v>-0.33652332307330102</v>
       </c>
     </row>
@@ -10915,49 +10915,49 @@
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
         <v>0.44422190783399301</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>-0.100484863596567</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>-3.6983458463896599E-2</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>-8.6008392193334504E-2</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>-0.12670777470059799</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="1">
         <v>-2.6511483695726298E-2</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
         <v>0.100266583577878</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="1">
         <v>0.124305525240195</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1">
         <v>-8.1070741633006704E-2</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="1">
         <v>-0.16006096719240701</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="1">
         <v>-0.28201325852252801</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="1">
         <v>-0.100481155347403</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="1">
         <v>-3.2513363121951903E-2</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="1">
         <v>-0.16005512529310401</v>
       </c>
     </row>
@@ -10968,49 +10968,49 @@
       <c r="B37" t="s">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>0.44422190783399301</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
         <v>-0.13547299368534901</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>-0.107512755430634</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>-6.7882990695107795E-2</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="1">
         <v>1.13399967942675E-2</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="1">
         <v>0.147809662499267</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
         <v>-1.0809869007547801E-2</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="1">
         <v>-8.6443183065445101E-2</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1">
         <v>6.4842711523723701E-2</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="1">
         <v>-0.12380742779394301</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="1">
         <v>-1.85038677390307E-3</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="1">
         <v>-0.13561104309820499</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="1">
         <v>-6.7735022415090607E-2</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="1">
         <v>-0.123809824447063</v>
       </c>
     </row>
@@ -11021,49 +11021,49 @@
       <c r="B38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
         <v>0.16715601774765501</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>-0.24018316227629699</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>-0.16845162422190499</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <v>-0.20633419008425799</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="1">
         <v>6.0317549130107902E-2</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="1">
         <v>0.28891277070312799</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="1">
         <v>-3.23149329578859E-2</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="1">
         <v>-0.14425286511577001</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1">
         <v>8.9729422885762702E-2</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="1">
         <v>-0.21312039626544799</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="1">
         <v>4.7033415423053303E-2</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="1">
         <v>-0.240105449891063</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="1">
         <v>-0.10532676765853</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="1">
         <v>-0.21312650503275701</v>
       </c>
     </row>
@@ -11074,49 +11074,49 @@
       <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>0.16715601774765501</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
         <v>-6.4443579026229894E-2</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>3.3063303722340402E-3</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <v>-3.3096759011707E-2</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="1">
         <v>2.34705899672151E-2</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="1">
         <v>6.1769695423432101E-2</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="1">
         <v>-3.5329985419809702E-2</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="1">
         <v>-3.43424358981173E-2</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1">
         <v>5.2172646109580299E-2</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="1">
         <v>-6.1505528305801499E-2</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="1">
         <v>-3.1204433450306601E-2</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="1">
         <v>-6.42391076526687E-2</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="1">
         <v>2.5654257784496402E-2</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="1">
         <v>-6.15026056136787E-2</v>
       </c>
     </row>

</xml_diff>